<commit_message>
Update readings to match table in paper
</commit_message>
<xml_diff>
--- a/Course_Schedule.xlsx
+++ b/Course_Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rnowling/Projects/csc6712-distributed-database-internals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rnowling/Projects/distributed-database-internals-course/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E53BA91-3FC0-DE47-9070-9266AE100C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF4AE3F-15B0-9345-9314-657CE5E51E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="760" windowWidth="28020" windowHeight="20320" xr2:uid="{FFCEDBB6-3965-344F-A10F-2524A45723A6}"/>
   </bookViews>
@@ -136,9 +136,6 @@
     <t>Transactions and Concurrency Control</t>
   </si>
   <si>
-    <t>DSC Ch. 23</t>
-  </si>
-  <si>
     <t>Distributed Transactions and Concurrency Control</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>DSC Ch. 19</t>
   </si>
   <si>
-    <t>DSC Ch. 17 - 18</t>
-  </si>
-  <si>
     <t>Week 16</t>
   </si>
   <si>
@@ -208,13 +202,19 @@
     <t>Recovery Systems</t>
   </si>
   <si>
-    <t>Junquiera 2011</t>
-  </si>
-  <si>
     <t>Consistency in Detail; Zab protocol</t>
   </si>
   <si>
     <t>CSApp Ch. 1, 6 (skip 6.4); DSC Ch. 12</t>
+  </si>
+  <si>
+    <t>DSC Ch. 17, 18.0 - 18.2, 18.8, 18.10</t>
+  </si>
+  <si>
+    <t>DSC Ch. 23.0 - 23.4 (skipping 23.2.3 - 23.3)</t>
+  </si>
+  <si>
+    <t>Junquiera 2011; DSC Ch. 23.6 - 23.9</t>
   </si>
 </sst>
 </file>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CFBD59-0614-5C4D-A4FB-BBEEF187C34D}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="155" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,13 +630,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -647,7 +647,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -658,7 +658,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -669,7 +669,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -677,7 +677,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -690,10 +690,10 @@
         <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -701,10 +701,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -718,7 +718,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -726,10 +726,10 @@
         <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -750,10 +750,10 @@
         <v>29</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -761,10 +761,10 @@
         <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -772,10 +772,10 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -783,10 +783,10 @@
         <v>11</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -804,13 +804,13 @@
         <v>12</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -818,7 +818,7 @@
         <v>13</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -831,7 +831,7 @@
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>27</v>

</xml_diff>